<commit_message>
Separado o menu do main
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -37,6 +37,519 @@
     <x:t>SALARY</x:t>
   </x:si>
   <x:si>
+    <x:t>Matthew</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Weiss</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MWEISS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.123.1234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ST_MAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Adam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fripp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AFRIPP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.123.2234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Payam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kaufling</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PKAUFLIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.123.3234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shanta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vollman</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SVOLLMAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.123.4234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kevin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mourgos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KMOURGOS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.123.5234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Julia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nayer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JNAYER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.1214</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ST_CLERK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Irene</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mikkilineni</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IMIKKILI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.1224</x:t>
+  </x:si>
+  <x:si>
+    <x:t>James</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Landry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JLANDRY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.1334</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Steven</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Markle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SMARKLE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.1434</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laura</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bissot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LBISSOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.5234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mozhe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Atkinson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MATKINSO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.6234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marlow</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JAMRLOW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.7234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TJ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Olson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TJOLSON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.124.8234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jason</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mallin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JMALLIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.127.1934</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Michael</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rogers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MROGERS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.127.1834</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ki</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KGEE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.127.1734</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hazel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Philtanker</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HPHILTAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.127.1634</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Renske</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ladwig</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RLADWIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.1234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stephen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stiles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSTILES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.2034</x:t>
+  </x:si>
+  <x:si>
+    <x:t>John</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Seo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JSEO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Joshua</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Patel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JPATEL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.1834</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trenna</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rajs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TRAJS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.8009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Curtis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Davies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CDAVIES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.2994</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Randall</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Matos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RMATOS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.2874</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Peter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vargas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PVARGAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.121.2004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Winston</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Taylor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WTAYLOR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SH_CLERK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jean</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fleaur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JFLEAUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9877</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Martha</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sullivan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSULLIVA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9878</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Girard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Geoni</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GGEONI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9879</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nandita</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sarchand</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NSARCHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.509.1876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alexis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bull</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ABULL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.509.2876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dellinger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JDELLING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.509.3876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anthony</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cabrio</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ACABRIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.509.4876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kelly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chung</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KCHUNG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.505.1876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jennifer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dilly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JDILLY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.505.2876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Timothy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gates</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TGATES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.505.3876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Perkins</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPERKINS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.505.4876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sarah</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bell</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SBELL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.501.1876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Britney</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Everett</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BEVERETT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.501.2876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Samuel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>McCain</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SMCCAIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.501.3876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jones</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VJONES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.501.4876</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Walsh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AWALSH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9811</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feeney</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KFEENEY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.507.9822</x:t>
+  </x:si>
+  <x:si>
     <x:t>Donald</x:t>
   </x:si>
   <x:si>
@@ -49,9 +562,6 @@
     <x:t>650.507.9833</x:t>
   </x:si>
   <x:si>
-    <x:t>SH_CLERK</x:t>
-  </x:si>
-  <x:si>
     <x:t>Douglas</x:t>
   </x:si>
   <x:si>
@@ -62,516 +572,6 @@
   </x:si>
   <x:si>
     <x:t>650.507.9844</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Matthew</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Weiss</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MWEISS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.123.1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ST_MAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Adam</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fripp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AFRIPP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.123.2234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payam</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kaufling</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PKAUFLIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.123.3234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shanta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vollman</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SVOLLMAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.123.4234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kevin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mourgos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KMOURGOS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.123.5234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Julia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nayer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JNAYER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.1214</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ST_CLERK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Irene</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mikkilineni</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IMIKKILI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.1224</x:t>
-  </x:si>
-  <x:si>
-    <x:t>James</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Landry</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JLANDRY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.1334</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Steven</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Markle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SMARKLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.1434</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laura</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bissot</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LBISSOT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.5234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mozhe</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Atkinson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MATKINSO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.6234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Marlow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JAMRLOW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.7234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Olson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TJOLSON</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.124.8234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jason</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mallin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JMALLIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.127.1934</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Michael</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rogers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MROGERS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.127.1834</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ki</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KGEE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.127.1734</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hazel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Philtanker</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HPHILTAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.127.1634</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Renske</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ladwig</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RLADWIG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stephen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stiles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSTILES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.2034</x:t>
-  </x:si>
-  <x:si>
-    <x:t>John</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Seo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JSEO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joshua</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JPATEL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.1834</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trenna</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rajs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRAJS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.8009</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Curtis</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Davies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CDAVIES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.2994</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Randall</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Matos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RMATOS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.2874</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Peter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vargas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PVARGAS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.121.2004</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Winston</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Taylor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WTAYLOR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jean</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fleaur</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JFLEAUR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9877</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Martha</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sullivan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSULLIVA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9878</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Girard</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Geoni</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GGEONI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9879</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nandita</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sarchand</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NSARCHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.509.1876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alexis</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bull</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ABULL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.509.2876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dellinger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JDELLING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.509.3876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Anthony</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cabrio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ACABRIO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.509.4876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kelly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chung</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KCHUNG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.505.1876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jennifer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dilly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JDILLY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.505.2876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Timothy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gates</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TGATES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.505.3876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Perkins</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPERKINS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.505.4876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sarah</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bell</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SBELL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.501.1876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Britney</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Everett</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BEVERETT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.501.2876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Samuel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>McCain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SMCCAIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.501.3876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jones</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VJONES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.501.4876</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Walsh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AWALSH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9811</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Feeney</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KFEENEY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>650.507.9822</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -959,7 +959,7 @@
     </x:row>
     <x:row r="2" spans="1:7">
       <x:c r="A2" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>7</x:v>
@@ -977,12 +977,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
-        <x:v>2600</x:v>
+        <x:v>8000</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
       <x:c r="A3" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>12</x:v>
@@ -1000,12 +1000,12 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
-        <x:v>2600</x:v>
+        <x:v>8200</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
       <x:c r="A4" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>16</x:v>
@@ -1020,84 +1020,84 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
-        <x:v>8000</x:v>
+        <x:v>7900</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="A5" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
+      <x:c r="E5" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
-        <x:v>8200</x:v>
+        <x:v>6500</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
-        <x:v>7900</x:v>
+        <x:v>5800</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="A7" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="D7" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="E7" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="E7" s="0" t="s">
+      <x:c r="F7" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
       <x:c r="G7" s="0" t="n">
-        <x:v>6500</x:v>
+        <x:v>3200</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
       <x:c r="A8" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>33</x:v>
@@ -1112,15 +1112,15 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
-        <x:v>5800</x:v>
+        <x:v>2700</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="A9" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>37</x:v>
@@ -1135,429 +1135,429 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
-        <x:v>3200</x:v>
+        <x:v>2400</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C10" s="0" t="s">
+      <x:c r="D10" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s">
+      <x:c r="E10" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>2700</x:v>
+        <x:v>2200</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="C11" s="0" t="s">
+      <x:c r="D11" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="E11" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>2400</x:v>
+        <x:v>3300</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C12" s="0" t="s">
+      <x:c r="D12" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D12" s="0" t="s">
+      <x:c r="E12" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
-        <x:v>2200</x:v>
+        <x:v>2800</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="C13" s="0" t="s">
+      <x:c r="E13" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
-        <x:v>3300</x:v>
+        <x:v>2500</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="C14" s="0" t="s">
+      <x:c r="E14" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
-        <x:v>2800</x:v>
+        <x:v>2100</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
       <x:c r="A15" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="D15" s="0" t="s">
+      <x:c r="E15" s="0" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
-        <x:v>2500</x:v>
+        <x:v>3300</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7">
       <x:c r="A16" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="C16" s="0" t="s">
+      <x:c r="D16" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="D16" s="0" t="s">
+      <x:c r="E16" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
-        <x:v>2100</x:v>
+        <x:v>2900</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
       <x:c r="A17" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
+      <x:c r="D17" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
+      <x:c r="E17" s="0" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
-        <x:v>3300</x:v>
+        <x:v>2400</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="A18" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="C18" s="0" t="s">
+      <x:c r="D18" s="0" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="E18" s="0" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
-        <x:v>2900</x:v>
+        <x:v>2200</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
       <x:c r="A19" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="C19" s="0" t="s">
+      <x:c r="D19" s="0" t="s">
         <x:v>78</x:v>
       </x:c>
-      <x:c r="D19" s="0" t="s">
+      <x:c r="E19" s="0" t="s">
         <x:v>79</x:v>
       </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>80</x:v>
-      </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
-        <x:v>2400</x:v>
+        <x:v>3600</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:7">
       <x:c r="A20" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="C20" s="0" t="s">
+      <x:c r="D20" s="0" t="s">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="D20" s="0" t="s">
+      <x:c r="E20" s="0" t="s">
         <x:v>83</x:v>
       </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
-        <x:v>2200</x:v>
+        <x:v>3200</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
       <x:c r="A21" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="C21" s="0" t="s">
+      <x:c r="D21" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
+      <x:c r="E21" s="0" t="s">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="E21" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
-        <x:v>3600</x:v>
+        <x:v>2700</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:7">
       <x:c r="A22" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="C22" s="0" t="s">
+      <x:c r="D22" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="D22" s="0" t="s">
+      <x:c r="E22" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="E22" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
-        <x:v>3200</x:v>
+        <x:v>2500</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:7">
       <x:c r="A23" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="C23" s="0" t="s">
+      <x:c r="D23" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="D23" s="0" t="s">
+      <x:c r="E23" s="0" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="E23" s="0" t="s">
-        <x:v>96</x:v>
-      </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
-        <x:v>2700</x:v>
+        <x:v>3500</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:7">
       <x:c r="A24" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="C24" s="0" t="s">
+      <x:c r="D24" s="0" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="D24" s="0" t="s">
+      <x:c r="E24" s="0" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
-        <x:v>2500</x:v>
+        <x:v>3100</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:7">
       <x:c r="A25" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
         <x:v>101</x:v>
       </x:c>
-      <x:c r="C25" s="0" t="s">
+      <x:c r="D25" s="0" t="s">
         <x:v>102</x:v>
       </x:c>
-      <x:c r="D25" s="0" t="s">
+      <x:c r="E25" s="0" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="E25" s="0" t="s">
-        <x:v>104</x:v>
-      </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
-        <x:v>3500</x:v>
+        <x:v>2600</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:7">
       <x:c r="A26" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="C26" s="0" t="s">
+      <x:c r="D26" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
-      <x:c r="D26" s="0" t="s">
+      <x:c r="E26" s="0" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>108</x:v>
-      </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
-        <x:v>3100</x:v>
+        <x:v>2500</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:7">
       <x:c r="A27" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
         <x:v>109</x:v>
       </x:c>
-      <x:c r="C27" s="0" t="s">
+      <x:c r="D27" s="0" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="D27" s="0" t="s">
+      <x:c r="E27" s="0" t="s">
         <x:v>111</x:v>
       </x:c>
-      <x:c r="E27" s="0" t="s">
+      <x:c r="F27" s="0" t="s">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="F27" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
       <x:c r="G27" s="0" t="n">
-        <x:v>2600</x:v>
+        <x:v>3200</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:7">
       <x:c r="A28" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
         <x:v>113</x:v>
@@ -1572,15 +1572,15 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
-        <x:v>2500</x:v>
+        <x:v>3100</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:7">
       <x:c r="A29" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
         <x:v>117</x:v>
@@ -1595,15 +1595,15 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
-        <x:v>3200</x:v>
+        <x:v>2500</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:7">
       <x:c r="A30" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
         <x:v>121</x:v>
@@ -1618,15 +1618,15 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
-        <x:v>3100</x:v>
+        <x:v>2800</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:7">
       <x:c r="A31" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
         <x:v>125</x:v>
@@ -1641,15 +1641,15 @@
         <x:v>128</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
-        <x:v>2500</x:v>
+        <x:v>4200</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:7">
       <x:c r="A32" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
         <x:v>129</x:v>
@@ -1664,64 +1664,64 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
-        <x:v>2800</x:v>
+        <x:v>4100</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:7">
       <x:c r="A33" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
         <x:v>133</x:v>
       </x:c>
-      <x:c r="C33" s="0" t="s">
+      <x:c r="D33" s="0" t="s">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="D33" s="0" t="s">
+      <x:c r="E33" s="0" t="s">
         <x:v>135</x:v>
       </x:c>
-      <x:c r="E33" s="0" t="s">
-        <x:v>136</x:v>
-      </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
-        <x:v>4200</x:v>
+        <x:v>3400</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:7">
       <x:c r="A34" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
         <x:v>137</x:v>
       </x:c>
-      <x:c r="C34" s="0" t="s">
+      <x:c r="D34" s="0" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="D34" s="0" t="s">
+      <x:c r="E34" s="0" t="s">
         <x:v>139</x:v>
       </x:c>
-      <x:c r="E34" s="0" t="s">
-        <x:v>140</x:v>
-      </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
-        <x:v>4100</x:v>
+        <x:v>3000</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:7">
       <x:c r="A35" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
         <x:v>141</x:v>
@@ -1733,15 +1733,15 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
-        <x:v>3400</x:v>
+        <x:v>3800</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7">
       <x:c r="A36" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
         <x:v>144</x:v>
@@ -1756,15 +1756,15 @@
         <x:v>147</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
-        <x:v>3000</x:v>
+        <x:v>3600</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7">
       <x:c r="A37" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
         <x:v>148</x:v>
@@ -1779,64 +1779,64 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
-        <x:v>3800</x:v>
+        <x:v>2900</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:7">
       <x:c r="A38" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
         <x:v>152</x:v>
       </x:c>
-      <x:c r="C38" s="0" t="s">
+      <x:c r="D38" s="0" t="s">
         <x:v>153</x:v>
       </x:c>
-      <x:c r="D38" s="0" t="s">
+      <x:c r="E38" s="0" t="s">
         <x:v>154</x:v>
       </x:c>
-      <x:c r="E38" s="0" t="s">
-        <x:v>155</x:v>
-      </x:c>
       <x:c r="F38" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
-        <x:v>3600</x:v>
+        <x:v>2500</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:7">
       <x:c r="A39" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
         <x:v>156</x:v>
       </x:c>
-      <x:c r="C39" s="0" t="s">
+      <x:c r="D39" s="0" t="s">
         <x:v>157</x:v>
       </x:c>
-      <x:c r="D39" s="0" t="s">
+      <x:c r="E39" s="0" t="s">
         <x:v>158</x:v>
       </x:c>
-      <x:c r="E39" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
       <x:c r="F39" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
-        <x:v>2900</x:v>
+        <x:v>4000</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:7">
       <x:c r="A40" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
         <x:v>160</x:v>
@@ -1848,15 +1848,15 @@
         <x:v>162</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
-        <x:v>2500</x:v>
+        <x:v>3900</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:7">
       <x:c r="A41" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
         <x:v>163</x:v>
@@ -1871,15 +1871,15 @@
         <x:v>166</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
-        <x:v>4000</x:v>
+        <x:v>3200</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:7">
       <x:c r="A42" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
         <x:v>167</x:v>
@@ -1894,15 +1894,15 @@
         <x:v>170</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
-        <x:v>3900</x:v>
+        <x:v>2800</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:7">
       <x:c r="A43" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
         <x:v>171</x:v>
@@ -1917,64 +1917,64 @@
         <x:v>174</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
-        <x:v>3200</x:v>
+        <x:v>3100</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:7">
       <x:c r="A44" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
         <x:v>175</x:v>
       </x:c>
-      <x:c r="C44" s="0" t="s">
+      <x:c r="D44" s="0" t="s">
         <x:v>176</x:v>
       </x:c>
-      <x:c r="D44" s="0" t="s">
+      <x:c r="E44" s="0" t="s">
         <x:v>177</x:v>
       </x:c>
-      <x:c r="E44" s="0" t="s">
-        <x:v>178</x:v>
-      </x:c>
       <x:c r="F44" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
-        <x:v>2800</x:v>
+        <x:v>3000</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:7">
       <x:c r="A45" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
         <x:v>179</x:v>
       </x:c>
-      <x:c r="C45" s="0" t="s">
+      <x:c r="D45" s="0" t="s">
         <x:v>180</x:v>
       </x:c>
-      <x:c r="D45" s="0" t="s">
+      <x:c r="E45" s="0" t="s">
         <x:v>181</x:v>
       </x:c>
-      <x:c r="E45" s="0" t="s">
-        <x:v>182</x:v>
-      </x:c>
       <x:c r="F45" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
-        <x:v>3100</x:v>
+        <x:v>2600</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:7">
       <x:c r="A46" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
         <x:v>183</x:v>
@@ -1986,10 +1986,10 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="F46" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
-        <x:v>3000</x:v>
+        <x:v>2600</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>